<commit_message>
Esta es la posta, ahora sí, sin los flash equivocados
</commit_message>
<xml_diff>
--- a/workspace/retinoblastomaSpringApp/dataPlusPlus.xlsx
+++ b/workspace/retinoblastomaSpringApp/dataPlusPlus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dataPlusPlus" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,14 @@
     <sheet name="positivos total" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataPlusPlus!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataPlusPlus!$A$1:$L$217</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="107">
   <si>
     <t>Archivo</t>
   </si>
@@ -340,6 +340,15 @@
   </si>
   <si>
     <t>Negativos automatico sin invalidos</t>
+  </si>
+  <si>
+    <t>promedio negativos total sin flash</t>
+  </si>
+  <si>
+    <t>promedio negativos optimo sin flash</t>
+  </si>
+  <si>
+    <t>promedio negativos automatico sin invalidos ni falsos ojos sin flash</t>
   </si>
 </sst>
 </file>
@@ -823,8 +832,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1192,16 +1202,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.4793416999999996E-2</c:v>
+                  <c:v>4.04401679375E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.278766603</c:v>
+                  <c:v>0.41007365427083298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59967446999999996</c:v>
+                  <c:v>0.51077074968750003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6765510000000001E-2</c:v>
+                  <c:v>3.8715428083333302E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2038,16 +2048,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.6197591999999995E-2</c:v>
+                  <c:v>9.7635686123077006E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33055579200000001</c:v>
+                  <c:v>0.33342090447692302</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56556237399999998</c:v>
+                  <c:v>0.53817678972307703</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7684242000000001E-2</c:v>
+                  <c:v>3.0766619692307699E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2440,16 +2450,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.59677833199999997</c:v>
+                  <c:v>0.64714692616666702</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26790805099999998</c:v>
+                  <c:v>0.233357719444444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9748431000000003E-2</c:v>
+                  <c:v>4.8191032777777802E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.5565186000000001E-2</c:v>
+                  <c:v>7.1304321611111096E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2842,16 +2852,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.72125704199999996</c:v>
+                  <c:v>0.725326338357143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17619155</c:v>
+                  <c:v>0.18696953033333299</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5554187000000001E-2</c:v>
+                  <c:v>3.47762381111111E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6997220999999996E-2</c:v>
+                  <c:v>6.3100991777777796E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3243,16 +3253,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.65736663799999995</c:v>
+                  <c:v>0.66940531336111098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.235868887</c:v>
+                  <c:v>0.23076964383333301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0324233000000003E-2</c:v>
+                  <c:v>4.6701759138888903E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6440242000000002E-2</c:v>
+                  <c:v>5.3123283666666701E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8316,10 +8326,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L236"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="A1:L1"/>
+    <sheetView topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="E230" sqref="E230:H230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8362,7 +8373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -8397,7 +8408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -8432,7 +8443,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -8458,7 +8469,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -8467,7 +8478,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -8493,7 +8504,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
         <v>16</v>
@@ -8502,7 +8513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -8540,7 +8551,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -8578,7 +8589,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -8616,7 +8627,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -8654,7 +8665,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -8689,7 +8700,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -8727,7 +8738,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -8765,7 +8776,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -8841,7 +8852,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -8917,7 +8928,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -8952,7 +8963,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -8987,7 +8998,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -9013,7 +9024,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J19" t="s">
         <v>16</v>
@@ -9022,7 +9033,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -9048,7 +9059,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J20" t="s">
         <v>13</v>
@@ -9057,7 +9068,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -9083,7 +9094,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J21" t="s">
         <v>16</v>
@@ -9095,7 +9106,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -9130,7 +9141,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -9165,7 +9176,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -9203,7 +9214,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -9241,7 +9252,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -9279,7 +9290,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -9317,7 +9328,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -9343,7 +9354,7 @@
         <v>0.16279069800000001</v>
       </c>
       <c r="I28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J28" t="s">
         <v>13</v>
@@ -9352,7 +9363,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -9378,7 +9389,7 @@
         <v>1.4492754E-2</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J29" t="s">
         <v>16</v>
@@ -9387,7 +9398,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -9422,7 +9433,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -9457,7 +9468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -9483,7 +9494,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
@@ -9492,7 +9503,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -9517,8 +9528,8 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33" t="s">
-        <v>16</v>
+      <c r="I33" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="J33" t="s">
         <v>13</v>
@@ -9527,7 +9538,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -9562,7 +9573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -9749,7 +9760,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -9787,7 +9798,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -9825,7 +9836,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -9863,7 +9874,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -9901,7 +9912,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -9936,7 +9947,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -9971,7 +9982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -10009,7 +10020,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -10047,7 +10058,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -10085,7 +10096,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -10123,7 +10134,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -10161,7 +10172,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -10199,7 +10210,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -10237,7 +10248,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -10272,7 +10283,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -10307,7 +10318,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -10342,7 +10353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -10377,7 +10388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -10409,7 +10420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
@@ -10444,7 +10455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -10476,7 +10487,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -10508,7 +10519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>37</v>
       </c>
@@ -10543,7 +10554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -10578,7 +10589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -10613,7 +10624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -10651,7 +10662,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -10689,7 +10700,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -10727,7 +10738,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -10765,7 +10776,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -10803,7 +10814,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -10841,7 +10852,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -10879,7 +10890,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -10917,7 +10928,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -10955,7 +10966,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>41</v>
       </c>
@@ -10990,7 +11001,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>41</v>
       </c>
@@ -11028,7 +11039,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -11066,7 +11077,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -11104,7 +11115,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -11142,7 +11153,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -11180,7 +11191,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>43</v>
       </c>
@@ -11215,7 +11226,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>43</v>
       </c>
@@ -11250,7 +11261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>44</v>
       </c>
@@ -11285,7 +11296,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>44</v>
       </c>
@@ -11323,7 +11334,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -11361,7 +11372,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>45</v>
       </c>
@@ -11399,7 +11410,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>45</v>
       </c>
@@ -11437,7 +11448,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>45</v>
       </c>
@@ -11475,7 +11486,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>45</v>
       </c>
@@ -11513,7 +11524,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>46</v>
       </c>
@@ -11548,7 +11559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>46</v>
       </c>
@@ -11583,7 +11594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>47</v>
       </c>
@@ -11618,7 +11629,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>47</v>
       </c>
@@ -11653,7 +11664,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -11688,7 +11699,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -11723,7 +11734,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>49</v>
       </c>
@@ -11758,7 +11769,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>49</v>
       </c>
@@ -11793,7 +11804,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>50</v>
       </c>
@@ -11831,7 +11842,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>50</v>
       </c>
@@ -11866,7 +11877,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>50</v>
       </c>
@@ -11904,7 +11915,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>51</v>
       </c>
@@ -11942,7 +11953,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>51</v>
       </c>
@@ -11980,7 +11991,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>51</v>
       </c>
@@ -12018,7 +12029,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -12056,7 +12067,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>51</v>
       </c>
@@ -12094,7 +12105,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>53</v>
       </c>
@@ -12129,7 +12140,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>53</v>
       </c>
@@ -12167,7 +12178,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>53</v>
       </c>
@@ -12205,7 +12216,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>54</v>
       </c>
@@ -12240,7 +12251,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>54</v>
       </c>
@@ -12278,7 +12289,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>54</v>
       </c>
@@ -12316,7 +12327,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>54</v>
       </c>
@@ -12757,7 +12768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>56</v>
       </c>
@@ -12783,7 +12794,7 @@
         <v>0</v>
       </c>
       <c r="I122" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J122" t="s">
         <v>16</v>
@@ -12795,7 +12806,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>56</v>
       </c>
@@ -12821,7 +12832,7 @@
         <v>0</v>
       </c>
       <c r="I123" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J123" t="s">
         <v>16</v>
@@ -12833,7 +12844,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>56</v>
       </c>
@@ -12859,7 +12870,7 @@
         <v>0</v>
       </c>
       <c r="I124" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J124" t="s">
         <v>16</v>
@@ -12871,7 +12882,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>56</v>
       </c>
@@ -12897,7 +12908,7 @@
         <v>0</v>
       </c>
       <c r="I125" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J125" t="s">
         <v>16</v>
@@ -12909,7 +12920,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>57</v>
       </c>
@@ -12947,7 +12958,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>57</v>
       </c>
@@ -12985,7 +12996,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>57</v>
       </c>
@@ -13023,7 +13034,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>57</v>
       </c>
@@ -13213,7 +13224,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -13248,7 +13259,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -13286,7 +13297,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -13321,7 +13332,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -14083,7 +14094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>63</v>
       </c>
@@ -14118,7 +14129,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>63</v>
       </c>
@@ -14521,7 +14532,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>67</v>
       </c>
@@ -14547,7 +14558,7 @@
         <v>0</v>
       </c>
       <c r="I170" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J170" t="s">
         <v>16</v>
@@ -14556,7 +14567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>67</v>
       </c>
@@ -14582,7 +14593,7 @@
         <v>0</v>
       </c>
       <c r="I171" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J171" t="s">
         <v>16</v>
@@ -14591,7 +14602,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>68</v>
       </c>
@@ -14629,7 +14640,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>68</v>
       </c>
@@ -14667,7 +14678,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>68</v>
       </c>
@@ -15155,7 +15166,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>71</v>
       </c>
@@ -15190,7 +15201,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>71</v>
       </c>
@@ -15225,7 +15236,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>71</v>
       </c>
@@ -15263,7 +15274,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>72</v>
       </c>
@@ -15301,7 +15312,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>72</v>
       </c>
@@ -15339,7 +15350,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>72</v>
       </c>
@@ -15377,7 +15388,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>72</v>
       </c>
@@ -15719,7 +15730,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>75</v>
       </c>
@@ -15754,7 +15765,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>75</v>
       </c>
@@ -15792,7 +15803,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>75</v>
       </c>
@@ -15982,7 +15993,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>77</v>
       </c>
@@ -16008,7 +16019,7 @@
         <v>0</v>
       </c>
       <c r="I209" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J209" t="s">
         <v>16</v>
@@ -16017,7 +16028,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>77</v>
       </c>
@@ -16043,7 +16054,7 @@
         <v>40</v>
       </c>
       <c r="I210" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J210" t="s">
         <v>16</v>
@@ -16055,7 +16066,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>77</v>
       </c>
@@ -16081,7 +16092,7 @@
         <v>0</v>
       </c>
       <c r="I211" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J211" t="s">
         <v>16</v>
@@ -16093,7 +16104,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>77</v>
       </c>
@@ -16119,7 +16130,7 @@
         <v>40</v>
       </c>
       <c r="I212" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J212" t="s">
         <v>16</v>
@@ -16131,7 +16142,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>78</v>
       </c>
@@ -16157,7 +16168,7 @@
         <v>0</v>
       </c>
       <c r="I213" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J213" t="s">
         <v>16</v>
@@ -16169,7 +16180,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>78</v>
       </c>
@@ -16195,7 +16206,7 @@
         <v>0</v>
       </c>
       <c r="I214" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J214" t="s">
         <v>16</v>
@@ -16207,7 +16218,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>78</v>
       </c>
@@ -16233,7 +16244,7 @@
         <v>0</v>
       </c>
       <c r="I215" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J215" t="s">
         <v>16</v>
@@ -16320,16 +16331,16 @@
         <v>80</v>
       </c>
       <c r="E219">
-        <v>0.65736663799999995</v>
+        <v>0.66940531336111098</v>
       </c>
       <c r="F219">
-        <v>0.235868887</v>
+        <v>0.23076964383333301</v>
       </c>
       <c r="G219">
-        <v>5.0324233000000003E-2</v>
+        <v>4.6701759138888903E-2</v>
       </c>
       <c r="H219">
-        <v>5.6440242000000002E-2</v>
+        <v>5.3123283666666701E-2</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.25">
@@ -16337,16 +16348,16 @@
         <v>81</v>
       </c>
       <c r="E220">
-        <v>0.72125704199999996</v>
+        <v>0.725326338357143</v>
       </c>
       <c r="F220">
-        <v>0.17619155</v>
+        <v>0.18696953033333299</v>
       </c>
       <c r="G220">
-        <v>3.5554187000000001E-2</v>
+        <v>3.47762381111111E-2</v>
       </c>
       <c r="H220">
-        <v>6.6997220999999996E-2</v>
+        <v>6.3100991777777796E-2</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.25">
@@ -16354,16 +16365,16 @@
         <v>82</v>
       </c>
       <c r="E221">
-        <v>0.59677833199999997</v>
+        <v>0.64714692616666702</v>
       </c>
       <c r="F221">
-        <v>0.26790805099999998</v>
+        <v>0.233357719444444</v>
       </c>
       <c r="G221">
-        <v>4.9748431000000003E-2</v>
+        <v>4.8191032777777802E-2</v>
       </c>
       <c r="H221">
-        <v>8.5565186000000001E-2</v>
+        <v>7.1304321611111096E-2</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.25">
@@ -16473,16 +16484,16 @@
         <v>89</v>
       </c>
       <c r="E228">
-        <v>7.6197591999999995E-2</v>
+        <v>8.3580043406249999E-2</v>
       </c>
       <c r="F228">
-        <v>0.33055579200000001</v>
+        <v>0.37172489226041699</v>
       </c>
       <c r="G228">
-        <v>0.56556237399999998</v>
+        <v>0.52118551906249999</v>
       </c>
       <c r="H228">
-        <v>2.7684242000000001E-2</v>
+        <v>2.3509545281249999E-2</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -16490,16 +16501,16 @@
         <v>90</v>
       </c>
       <c r="E229">
-        <v>8.4793416999999996E-2</v>
+        <v>9.7635686123077006E-2</v>
       </c>
       <c r="F229">
-        <v>0.278766603</v>
+        <v>0.33342090447692302</v>
       </c>
       <c r="G229">
-        <v>0.59967446999999996</v>
+        <v>0.53817678972307703</v>
       </c>
       <c r="H229">
-        <v>3.6765510000000001E-2</v>
+        <v>3.0766619692307699E-2</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -16507,16 +16518,16 @@
         <v>91</v>
       </c>
       <c r="E230">
-        <v>4.2905379E-2</v>
+        <v>4.04401679375E-2</v>
       </c>
       <c r="F230">
-        <v>0.35823069200000002</v>
+        <v>0.41007365427083298</v>
       </c>
       <c r="G230">
-        <v>0.55564670699999996</v>
+        <v>0.51077074968750003</v>
       </c>
       <c r="H230">
-        <v>4.3217222E-2</v>
+        <v>3.8715428083333302E-2</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -16621,9 +16632,72 @@
         <v>0.80555555599999995</v>
       </c>
     </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>104</v>
+      </c>
+      <c r="E237">
+        <v>1.6954083184210499E-2</v>
+      </c>
+      <c r="F237">
+        <v>0.82586733143421098</v>
+      </c>
+      <c r="G237">
+        <v>0.15546026456578901</v>
+      </c>
+      <c r="H237">
+        <v>1.71832081578947E-3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>105</v>
+      </c>
+      <c r="E238">
+        <v>3.5221119512195099E-3</v>
+      </c>
+      <c r="F238">
+        <v>0.90724193778048801</v>
+      </c>
+      <c r="G238">
+        <v>8.8527737365853704E-2</v>
+      </c>
+      <c r="H238">
+        <v>7.0821290243902396E-4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>106</v>
+      </c>
+      <c r="E239">
+        <v>4.6249107045454499E-2</v>
+      </c>
+      <c r="F239">
+        <v>0.87127833072727301</v>
+      </c>
+      <c r="G239">
+        <v>7.7856396181818194E-2</v>
+      </c>
+      <c r="H239">
+        <v>4.6161660454545504E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:L217">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="false"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="false"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16631,8 +16705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16656,16 +16730,16 @@
         <v>103</v>
       </c>
       <c r="B2">
-        <v>8.4793416999999996E-2</v>
+        <v>4.04401679375E-2</v>
       </c>
       <c r="C2">
-        <v>0.278766603</v>
+        <v>0.41007365427083298</v>
       </c>
       <c r="D2">
-        <v>0.59967446999999996</v>
+        <v>0.51077074968750003</v>
       </c>
       <c r="E2">
-        <v>3.6765510000000001E-2</v>
+        <v>3.8715428083333302E-2</v>
       </c>
     </row>
   </sheetData>
@@ -16679,7 +16753,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16726,7 +16800,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16750,16 +16824,16 @@
         <v>101</v>
       </c>
       <c r="B2">
-        <v>7.6197591999999995E-2</v>
+        <v>9.7635686123077006E-2</v>
       </c>
       <c r="C2">
-        <v>0.33055579200000001</v>
+        <v>0.33342090447692302</v>
       </c>
       <c r="D2">
-        <v>0.56556237399999998</v>
+        <v>0.53817678972307703</v>
       </c>
       <c r="E2">
-        <v>2.7684242000000001E-2</v>
+        <v>3.0766619692307699E-2</v>
       </c>
     </row>
   </sheetData>
@@ -16773,7 +16847,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16797,16 +16871,16 @@
         <v>99</v>
       </c>
       <c r="B2">
-        <v>0.59677833199999997</v>
+        <v>0.64714692616666702</v>
       </c>
       <c r="C2">
-        <v>0.26790805099999998</v>
+        <v>0.233357719444444</v>
       </c>
       <c r="D2">
-        <v>4.9748431000000003E-2</v>
+        <v>4.8191032777777802E-2</v>
       </c>
       <c r="E2">
-        <v>8.5565186000000001E-2</v>
+        <v>7.1304321611111096E-2</v>
       </c>
     </row>
   </sheetData>
@@ -16820,7 +16894,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16844,16 +16918,16 @@
         <v>98</v>
       </c>
       <c r="B2">
-        <v>0.72125704199999996</v>
+        <v>0.725326338357143</v>
       </c>
       <c r="C2">
-        <v>0.17619155</v>
+        <v>0.18696953033333299</v>
       </c>
       <c r="D2">
-        <v>3.5554187000000001E-2</v>
+        <v>3.47762381111111E-2</v>
       </c>
       <c r="E2">
-        <v>6.6997220999999996E-2</v>
+        <v>6.3100991777777796E-2</v>
       </c>
     </row>
   </sheetData>
@@ -16867,7 +16941,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16891,16 +16965,16 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>0.65736663799999995</v>
+        <v>0.66940531336111098</v>
       </c>
       <c r="C2">
-        <v>0.235868887</v>
+        <v>0.23076964383333301</v>
       </c>
       <c r="D2">
-        <v>5.0324233000000003E-2</v>
+        <v>4.6701759138888903E-2</v>
       </c>
       <c r="E2">
-        <v>5.6440242000000002E-2</v>
+        <v>5.3123283666666701E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Acomodados títulos de los gráficos para usarlos en el informe
</commit_message>
<xml_diff>
--- a/workspace/retinoblastomaSpringApp/dataPlusPlus.xlsx
+++ b/workspace/retinoblastomaSpringApp/dataPlusPlus.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\retinoblastoma\workspace\retinoblastomaSpringApp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="dataPlusPlus" sheetId="1" r:id="rId1"/>
@@ -837,48 +832,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -896,7 +891,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -909,7 +904,56 @@
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400"/>
+              <a:t>Detección automática</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400" baseline="0"/>
+              <a:t> en casos </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>negativos</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR" sz="1400" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11734711286089239"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -918,32 +962,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1319,7 +1337,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1332,6 +1350,37 @@
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400"/>
+              <a:t>Detección óptima en casos negativos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1341,32 +1390,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1742,7 +1765,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1755,6 +1778,42 @@
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400"/>
+              <a:t>Detecciones totales en casos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400" baseline="0"/>
+              <a:t> negativos</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1764,32 +1823,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2165,7 +2198,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2178,6 +2211,42 @@
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400"/>
+              <a:t>Detección automática en</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400" baseline="0"/>
+              <a:t> casos positivos</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2187,32 +2256,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2567,7 +2610,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2580,6 +2623,37 @@
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400"/>
+              <a:t>Detección óptima en casos positivos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2589,32 +2663,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2969,7 +3017,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2981,6 +3029,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400"/>
+              <a:t>Detecciones totales en casos positivos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2990,32 +3069,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3367,3222 +3420,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6846,7 +3683,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6881,7 +3718,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7058,7 +3895,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8329,11 +5166,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="O58" sqref="O58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -16701,10 +13538,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -16748,10 +13585,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -16795,10 +13632,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -16842,10 +13679,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -16889,10 +13726,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -16935,11 +13772,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
Agregadas columnas de resultados por criterio
</commit_message>
<xml_diff>
--- a/workspace/retinoblastomaSpringApp/dataPlusPlus.xlsx
+++ b/workspace/retinoblastomaSpringApp/dataPlusPlus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="dataPlusPlus" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,14 @@
     <sheet name="positivos total" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataPlusPlus!$A$1:$L$217</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataPlusPlus!$A$1:$O$217</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="112">
   <si>
     <t>Archivo</t>
   </si>
@@ -344,6 +344,21 @@
   </si>
   <si>
     <t>promedio negativos automatico sin invalidos ni falsos ojos sin flash</t>
+  </si>
+  <si>
+    <t>Criterio 1</t>
+  </si>
+  <si>
+    <t>Criterio 2</t>
+  </si>
+  <si>
+    <t>Criterio 3</t>
+  </si>
+  <si>
+    <t>Negativo</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -832,48 +847,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1257,7 +1272,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1814,7 +1828,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2118,7 +2131,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2247,7 +2259,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2530,7 +2541,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2654,7 +2664,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2937,7 +2946,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3895,7 +3903,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5164,15 +5172,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L239"/>
+  <dimension ref="A1:O239"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="O58" sqref="O58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5209,8 +5217,17 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5245,7 +5262,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5280,7 +5297,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -5315,7 +5332,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -5350,7 +5367,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5387,8 +5404,17 @@
       <c r="L6">
         <v>161</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>110</v>
+      </c>
+      <c r="N6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -5425,8 +5451,17 @@
       <c r="L7">
         <v>161</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N7" t="s">
+        <v>110</v>
+      </c>
+      <c r="O7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -5464,7 +5499,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -5502,7 +5537,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -5536,8 +5571,17 @@
       <c r="L10">
         <v>382</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5574,8 +5618,17 @@
       <c r="L11">
         <v>382</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>110</v>
+      </c>
+      <c r="N11" t="s">
+        <v>110</v>
+      </c>
+      <c r="O11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -5613,7 +5666,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -5651,7 +5704,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -5689,7 +5742,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -5727,7 +5780,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -5765,7 +5818,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -5799,8 +5852,17 @@
       <c r="L17">
         <v>366</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -5834,8 +5896,17 @@
       <c r="L18">
         <v>366</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>110</v>
+      </c>
+      <c r="N18" t="s">
+        <v>110</v>
+      </c>
+      <c r="O18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -5869,8 +5940,17 @@
       <c r="L19">
         <v>730</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>110</v>
+      </c>
+      <c r="N19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -5904,8 +5984,17 @@
       <c r="L20">
         <v>730</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" t="s">
+        <v>9</v>
+      </c>
+      <c r="O20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -5942,8 +6031,17 @@
       <c r="L21">
         <v>730</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>110</v>
+      </c>
+      <c r="N21" t="s">
+        <v>110</v>
+      </c>
+      <c r="O21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -5977,8 +6075,17 @@
       <c r="L22">
         <v>529</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>110</v>
+      </c>
+      <c r="N22" t="s">
+        <v>110</v>
+      </c>
+      <c r="O22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -6012,8 +6119,17 @@
       <c r="L23">
         <v>529</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -6050,8 +6166,17 @@
       <c r="L24">
         <v>313</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6088,8 +6213,17 @@
       <c r="L25">
         <v>313</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>110</v>
+      </c>
+      <c r="N25" t="s">
+        <v>110</v>
+      </c>
+      <c r="O25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -6127,7 +6261,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -6165,7 +6299,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -6200,7 +6334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -6235,7 +6369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -6270,7 +6404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -6305,7 +6439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -6339,8 +6473,17 @@
       <c r="L32">
         <v>304</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -6374,8 +6517,17 @@
       <c r="L33">
         <v>304</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -6410,7 +6562,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -6445,7 +6597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -6483,7 +6635,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -6521,7 +6673,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -6559,7 +6711,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -6597,7 +6749,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -6634,8 +6786,17 @@
       <c r="L40">
         <v>550</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>110</v>
+      </c>
+      <c r="N40" t="s">
+        <v>110</v>
+      </c>
+      <c r="O40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -6672,8 +6833,17 @@
       <c r="L41">
         <v>550</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>9</v>
+      </c>
+      <c r="N41" t="s">
+        <v>9</v>
+      </c>
+      <c r="O41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -6711,7 +6881,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -6749,7 +6919,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -6784,7 +6954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -6819,7 +6989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -6856,8 +7026,17 @@
       <c r="L46">
         <v>177</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" t="s">
+        <v>9</v>
+      </c>
+      <c r="O46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -6895,7 +7074,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -6933,7 +7112,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -6970,8 +7149,17 @@
       <c r="L49">
         <v>384</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>9</v>
+      </c>
+      <c r="N49" t="s">
+        <v>9</v>
+      </c>
+      <c r="O49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -7008,8 +7196,17 @@
       <c r="L50">
         <v>384</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>110</v>
+      </c>
+      <c r="N50" t="s">
+        <v>110</v>
+      </c>
+      <c r="O50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -7047,7 +7244,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -7085,7 +7282,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -7119,8 +7316,17 @@
       <c r="L53">
         <v>1002</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M53" t="s">
+        <v>110</v>
+      </c>
+      <c r="N53" t="s">
+        <v>110</v>
+      </c>
+      <c r="O53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -7154,8 +7360,17 @@
       <c r="L54">
         <v>1002</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M54" t="s">
+        <v>110</v>
+      </c>
+      <c r="N54" t="s">
+        <v>110</v>
+      </c>
+      <c r="O54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -7189,8 +7404,17 @@
       <c r="K55" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M55" t="s">
+        <v>110</v>
+      </c>
+      <c r="N55" t="s">
+        <v>110</v>
+      </c>
+      <c r="O55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -7224,8 +7448,17 @@
       <c r="K56" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M56" t="s">
+        <v>110</v>
+      </c>
+      <c r="N56" t="s">
+        <v>110</v>
+      </c>
+      <c r="O56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -7256,8 +7489,17 @@
       <c r="J57" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57" t="s">
+        <v>110</v>
+      </c>
+      <c r="N57" t="s">
+        <v>110</v>
+      </c>
+      <c r="O57" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
@@ -7291,8 +7533,17 @@
       <c r="K58" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M58" t="s">
+        <v>9</v>
+      </c>
+      <c r="N58" t="s">
+        <v>9</v>
+      </c>
+      <c r="O58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -7323,8 +7574,17 @@
       <c r="J59" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M59" t="s">
+        <v>110</v>
+      </c>
+      <c r="N59" t="s">
+        <v>110</v>
+      </c>
+      <c r="O59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -7355,8 +7615,17 @@
       <c r="J60" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M60" t="s">
+        <v>110</v>
+      </c>
+      <c r="N60" t="s">
+        <v>110</v>
+      </c>
+      <c r="O60" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>37</v>
       </c>
@@ -7391,7 +7660,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -7426,7 +7695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -7461,7 +7730,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -7498,8 +7767,17 @@
       <c r="L64">
         <v>231</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M64" t="s">
+        <v>9</v>
+      </c>
+      <c r="N64" t="s">
+        <v>9</v>
+      </c>
+      <c r="O64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -7536,8 +7814,17 @@
       <c r="L65">
         <v>231</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65" t="s">
+        <v>110</v>
+      </c>
+      <c r="N65" t="s">
+        <v>110</v>
+      </c>
+      <c r="O65" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -7574,8 +7861,17 @@
       <c r="L66">
         <v>256</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M66" t="s">
+        <v>111</v>
+      </c>
+      <c r="N66" t="s">
+        <v>111</v>
+      </c>
+      <c r="O66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -7612,8 +7908,17 @@
       <c r="L67">
         <v>256</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M67" t="s">
+        <v>110</v>
+      </c>
+      <c r="N67" t="s">
+        <v>110</v>
+      </c>
+      <c r="O67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -7651,7 +7956,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -7689,7 +7994,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -7727,7 +8032,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -7765,7 +8070,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -7802,8 +8107,17 @@
       <c r="L72">
         <v>367</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72" t="s">
+        <v>110</v>
+      </c>
+      <c r="N72" t="s">
+        <v>110</v>
+      </c>
+      <c r="O72" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>41</v>
       </c>
@@ -7837,8 +8151,17 @@
       <c r="L73">
         <v>367</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M73" t="s">
+        <v>9</v>
+      </c>
+      <c r="N73" t="s">
+        <v>9</v>
+      </c>
+      <c r="O73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>41</v>
       </c>
@@ -7876,7 +8199,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -7913,8 +8236,17 @@
       <c r="L75">
         <v>185</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M75" t="s">
+        <v>110</v>
+      </c>
+      <c r="N75" t="s">
+        <v>110</v>
+      </c>
+      <c r="O75" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -7951,8 +8283,17 @@
       <c r="L76">
         <v>185</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M76" t="s">
+        <v>110</v>
+      </c>
+      <c r="N76" t="s">
+        <v>110</v>
+      </c>
+      <c r="O76" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -7990,7 +8331,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -8028,7 +8369,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>43</v>
       </c>
@@ -8063,7 +8404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>43</v>
       </c>
@@ -8098,7 +8439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>44</v>
       </c>
@@ -8132,8 +8473,17 @@
       <c r="L81">
         <v>272</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M81" t="s">
+        <v>9</v>
+      </c>
+      <c r="N81" t="s">
+        <v>9</v>
+      </c>
+      <c r="O81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>44</v>
       </c>
@@ -8170,8 +8520,17 @@
       <c r="L82">
         <v>272</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M82" t="s">
+        <v>110</v>
+      </c>
+      <c r="N82" t="s">
+        <v>110</v>
+      </c>
+      <c r="O82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -8209,7 +8568,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>45</v>
       </c>
@@ -8246,8 +8605,17 @@
       <c r="L84">
         <v>252</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M84" t="s">
+        <v>110</v>
+      </c>
+      <c r="N84" t="s">
+        <v>110</v>
+      </c>
+      <c r="O84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>45</v>
       </c>
@@ -8284,8 +8652,17 @@
       <c r="L85">
         <v>252</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M85" t="s">
+        <v>110</v>
+      </c>
+      <c r="N85" t="s">
+        <v>110</v>
+      </c>
+      <c r="O85" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>45</v>
       </c>
@@ -8323,7 +8700,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>45</v>
       </c>
@@ -8361,7 +8738,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>46</v>
       </c>
@@ -8396,7 +8773,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>46</v>
       </c>
@@ -8431,7 +8808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>47</v>
       </c>
@@ -8465,8 +8842,17 @@
       <c r="L90">
         <v>617</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M90" t="s">
+        <v>9</v>
+      </c>
+      <c r="N90" t="s">
+        <v>9</v>
+      </c>
+      <c r="O90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>47</v>
       </c>
@@ -8500,8 +8886,17 @@
       <c r="L91">
         <v>617</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M91" t="s">
+        <v>110</v>
+      </c>
+      <c r="N91" t="s">
+        <v>110</v>
+      </c>
+      <c r="O91" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -8536,7 +8931,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -8571,7 +8966,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>49</v>
       </c>
@@ -8605,8 +9000,17 @@
       <c r="L94">
         <v>1266</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M94" t="s">
+        <v>9</v>
+      </c>
+      <c r="N94" t="s">
+        <v>9</v>
+      </c>
+      <c r="O94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>49</v>
       </c>
@@ -8640,8 +9044,17 @@
       <c r="L95">
         <v>1266</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M95" t="s">
+        <v>110</v>
+      </c>
+      <c r="N95" t="s">
+        <v>110</v>
+      </c>
+      <c r="O95" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>50</v>
       </c>
@@ -8678,8 +9091,17 @@
       <c r="L96">
         <v>217</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M96" t="s">
+        <v>110</v>
+      </c>
+      <c r="N96" t="s">
+        <v>110</v>
+      </c>
+      <c r="O96" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>50</v>
       </c>
@@ -8713,8 +9135,17 @@
       <c r="L97">
         <v>217</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M97" t="s">
+        <v>110</v>
+      </c>
+      <c r="N97" t="s">
+        <v>110</v>
+      </c>
+      <c r="O97" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>50</v>
       </c>
@@ -8752,7 +9183,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>51</v>
       </c>
@@ -8789,8 +9220,17 @@
       <c r="L99">
         <v>280</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M99" t="s">
+        <v>110</v>
+      </c>
+      <c r="N99" t="s">
+        <v>110</v>
+      </c>
+      <c r="O99" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>51</v>
       </c>
@@ -8827,8 +9267,17 @@
       <c r="L100">
         <v>280</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M100" t="s">
+        <v>110</v>
+      </c>
+      <c r="N100" t="s">
+        <v>110</v>
+      </c>
+      <c r="O100" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>51</v>
       </c>
@@ -8865,8 +9314,17 @@
       <c r="L101">
         <v>280</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M101" t="s">
+        <v>111</v>
+      </c>
+      <c r="N101" t="s">
+        <v>111</v>
+      </c>
+      <c r="O101" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -8904,7 +9362,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>51</v>
       </c>
@@ -8942,7 +9400,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>53</v>
       </c>
@@ -8976,8 +9434,17 @@
       <c r="L104">
         <v>211</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M104" t="s">
+        <v>110</v>
+      </c>
+      <c r="N104" t="s">
+        <v>110</v>
+      </c>
+      <c r="O104" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>53</v>
       </c>
@@ -9014,8 +9481,17 @@
       <c r="L105">
         <v>211</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M105" t="s">
+        <v>110</v>
+      </c>
+      <c r="N105" t="s">
+        <v>110</v>
+      </c>
+      <c r="O105" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>53</v>
       </c>
@@ -9053,7 +9529,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>54</v>
       </c>
@@ -9087,8 +9563,17 @@
       <c r="L107">
         <v>794</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M107" t="s">
+        <v>110</v>
+      </c>
+      <c r="N107" t="s">
+        <v>110</v>
+      </c>
+      <c r="O107" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>54</v>
       </c>
@@ -9125,8 +9610,17 @@
       <c r="L108">
         <v>794</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M108" t="s">
+        <v>110</v>
+      </c>
+      <c r="N108" t="s">
+        <v>110</v>
+      </c>
+      <c r="O108" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>54</v>
       </c>
@@ -9163,8 +9657,17 @@
       <c r="L109">
         <v>794</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M109" t="s">
+        <v>111</v>
+      </c>
+      <c r="N109" t="s">
+        <v>111</v>
+      </c>
+      <c r="O109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>54</v>
       </c>
@@ -9202,7 +9705,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>55</v>
       </c>
@@ -9240,7 +9743,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>55</v>
       </c>
@@ -9278,7 +9781,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>55</v>
       </c>
@@ -9316,7 +9819,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>55</v>
       </c>
@@ -9354,7 +9857,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>55</v>
       </c>
@@ -9392,7 +9895,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>55</v>
       </c>
@@ -9430,7 +9933,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>55</v>
       </c>
@@ -9465,7 +9968,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>55</v>
       </c>
@@ -9500,7 +10003,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>55</v>
       </c>
@@ -9535,7 +10038,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>55</v>
       </c>
@@ -9570,7 +10073,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>55</v>
       </c>
@@ -9605,7 +10108,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>56</v>
       </c>
@@ -9642,8 +10145,17 @@
       <c r="L122">
         <v>366</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M122" t="s">
+        <v>110</v>
+      </c>
+      <c r="N122" t="s">
+        <v>110</v>
+      </c>
+      <c r="O122" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>56</v>
       </c>
@@ -9680,8 +10192,17 @@
       <c r="L123">
         <v>366</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M123" t="s">
+        <v>110</v>
+      </c>
+      <c r="N123" t="s">
+        <v>110</v>
+      </c>
+      <c r="O123" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>56</v>
       </c>
@@ -9719,7 +10240,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>56</v>
       </c>
@@ -9757,7 +10278,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>57</v>
       </c>
@@ -9794,8 +10315,17 @@
       <c r="L126">
         <v>301</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M126" t="s">
+        <v>110</v>
+      </c>
+      <c r="N126" t="s">
+        <v>110</v>
+      </c>
+      <c r="O126" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>57</v>
       </c>
@@ -9832,8 +10362,17 @@
       <c r="L127">
         <v>301</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M127" t="s">
+        <v>110</v>
+      </c>
+      <c r="N127" t="s">
+        <v>110</v>
+      </c>
+      <c r="O127" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>57</v>
       </c>
@@ -9871,7 +10410,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>57</v>
       </c>
@@ -9909,7 +10448,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>58</v>
       </c>
@@ -9947,7 +10486,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>58</v>
       </c>
@@ -9985,7 +10524,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>58</v>
       </c>
@@ -10023,7 +10562,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>58</v>
       </c>
@@ -10061,7 +10600,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -10095,8 +10634,17 @@
       <c r="L134">
         <v>322</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M134" t="s">
+        <v>110</v>
+      </c>
+      <c r="N134" t="s">
+        <v>110</v>
+      </c>
+      <c r="O134" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -10133,8 +10681,17 @@
       <c r="L135">
         <v>322</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M135" t="s">
+        <v>110</v>
+      </c>
+      <c r="N135" t="s">
+        <v>110</v>
+      </c>
+      <c r="O135" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -10168,8 +10725,17 @@
       <c r="L136">
         <v>322</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M136" t="s">
+        <v>9</v>
+      </c>
+      <c r="N136" t="s">
+        <v>110</v>
+      </c>
+      <c r="O136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -10207,7 +10773,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>60</v>
       </c>
@@ -10242,7 +10808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>60</v>
       </c>
@@ -10277,7 +10843,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>61</v>
       </c>
@@ -10312,7 +10878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>61</v>
       </c>
@@ -10347,7 +10913,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>62</v>
       </c>
@@ -10385,7 +10951,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>62</v>
       </c>
@@ -10423,7 +10989,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>62</v>
       </c>
@@ -10461,7 +11027,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>62</v>
       </c>
@@ -10499,7 +11065,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>62</v>
       </c>
@@ -10537,7 +11103,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>62</v>
       </c>
@@ -10575,7 +11141,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>62</v>
       </c>
@@ -10613,7 +11179,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>62</v>
       </c>
@@ -10651,7 +11217,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>62</v>
       </c>
@@ -10686,7 +11252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>62</v>
       </c>
@@ -10721,7 +11287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>62</v>
       </c>
@@ -10756,7 +11322,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>62</v>
       </c>
@@ -10791,7 +11357,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>62</v>
       </c>
@@ -10826,7 +11392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -10861,7 +11427,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>62</v>
       </c>
@@ -10896,7 +11462,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>62</v>
       </c>
@@ -10931,7 +11497,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>63</v>
       </c>
@@ -10965,8 +11531,17 @@
       <c r="L158">
         <v>850</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M158" t="s">
+        <v>110</v>
+      </c>
+      <c r="N158" t="s">
+        <v>110</v>
+      </c>
+      <c r="O158" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>63</v>
       </c>
@@ -11000,8 +11575,17 @@
       <c r="L159">
         <v>850</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M159" t="s">
+        <v>110</v>
+      </c>
+      <c r="N159" t="s">
+        <v>110</v>
+      </c>
+      <c r="O159" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>64</v>
       </c>
@@ -11039,7 +11623,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>64</v>
       </c>
@@ -11077,7 +11661,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>64</v>
       </c>
@@ -11115,7 +11699,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>64</v>
       </c>
@@ -11153,7 +11737,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>64</v>
       </c>
@@ -11191,7 +11775,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>64</v>
       </c>
@@ -11229,7 +11813,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>65</v>
       </c>
@@ -11264,7 +11848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>65</v>
       </c>
@@ -11299,7 +11883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>66</v>
       </c>
@@ -11334,7 +11918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>66</v>
       </c>
@@ -11369,7 +11953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>67</v>
       </c>
@@ -11404,7 +11988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>67</v>
       </c>
@@ -11439,7 +12023,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>68</v>
       </c>
@@ -11476,8 +12060,17 @@
       <c r="L172">
         <v>422</v>
       </c>
-    </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M172" t="s">
+        <v>110</v>
+      </c>
+      <c r="N172" t="s">
+        <v>110</v>
+      </c>
+      <c r="O172" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>68</v>
       </c>
@@ -11515,7 +12108,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>68</v>
       </c>
@@ -11553,7 +12146,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>69</v>
       </c>
@@ -11591,7 +12184,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>69</v>
       </c>
@@ -11629,7 +12222,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>69</v>
       </c>
@@ -11667,7 +12260,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>69</v>
       </c>
@@ -11705,7 +12298,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>70</v>
       </c>
@@ -11743,7 +12336,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>70</v>
       </c>
@@ -11781,7 +12374,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>70</v>
       </c>
@@ -11819,7 +12412,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>70</v>
       </c>
@@ -11857,7 +12450,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>70</v>
       </c>
@@ -11895,7 +12488,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>70</v>
       </c>
@@ -11933,7 +12526,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>70</v>
       </c>
@@ -11968,7 +12561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>70</v>
       </c>
@@ -12003,7 +12596,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>71</v>
       </c>
@@ -12037,8 +12630,17 @@
       <c r="L187">
         <v>685</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M187" t="s">
+        <v>110</v>
+      </c>
+      <c r="N187" t="s">
+        <v>110</v>
+      </c>
+      <c r="O187" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>71</v>
       </c>
@@ -12072,8 +12674,17 @@
       <c r="L188">
         <v>685</v>
       </c>
-    </row>
-    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M188" t="s">
+        <v>110</v>
+      </c>
+      <c r="N188" t="s">
+        <v>110</v>
+      </c>
+      <c r="O188" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>71</v>
       </c>
@@ -12110,8 +12721,17 @@
       <c r="L189">
         <v>685</v>
       </c>
-    </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M189" t="s">
+        <v>110</v>
+      </c>
+      <c r="N189" t="s">
+        <v>110</v>
+      </c>
+      <c r="O189" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>72</v>
       </c>
@@ -12148,8 +12768,17 @@
       <c r="L190">
         <v>331</v>
       </c>
-    </row>
-    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M190" t="s">
+        <v>110</v>
+      </c>
+      <c r="N190" t="s">
+        <v>110</v>
+      </c>
+      <c r="O190" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>72</v>
       </c>
@@ -12186,8 +12815,17 @@
       <c r="L191">
         <v>331</v>
       </c>
-    </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M191" t="s">
+        <v>110</v>
+      </c>
+      <c r="N191" t="s">
+        <v>110</v>
+      </c>
+      <c r="O191" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>72</v>
       </c>
@@ -12225,7 +12863,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>72</v>
       </c>
@@ -12263,7 +12901,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>73</v>
       </c>
@@ -12301,7 +12939,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>73</v>
       </c>
@@ -12339,7 +12977,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>73</v>
       </c>
@@ -12377,7 +13015,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>73</v>
       </c>
@@ -12415,7 +13053,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>74</v>
       </c>
@@ -12453,7 +13091,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>74</v>
       </c>
@@ -12491,7 +13129,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>74</v>
       </c>
@@ -12529,7 +13167,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>74</v>
       </c>
@@ -12567,7 +13205,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>75</v>
       </c>
@@ -12601,8 +13239,17 @@
       <c r="L202">
         <v>546</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M202" t="s">
+        <v>9</v>
+      </c>
+      <c r="N202" t="s">
+        <v>9</v>
+      </c>
+      <c r="O202" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>75</v>
       </c>
@@ -12639,8 +13286,17 @@
       <c r="L203">
         <v>546</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M203" t="s">
+        <v>110</v>
+      </c>
+      <c r="N203" t="s">
+        <v>110</v>
+      </c>
+      <c r="O203" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>75</v>
       </c>
@@ -12678,7 +13334,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>76</v>
       </c>
@@ -12716,7 +13372,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>76</v>
       </c>
@@ -12754,7 +13410,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>76</v>
       </c>
@@ -12792,7 +13448,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>76</v>
       </c>
@@ -12830,7 +13486,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>77</v>
       </c>
@@ -12864,8 +13520,17 @@
       <c r="L209">
         <v>338</v>
       </c>
-    </row>
-    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M209" t="s">
+        <v>110</v>
+      </c>
+      <c r="N209" t="s">
+        <v>110</v>
+      </c>
+      <c r="O209" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>77</v>
       </c>
@@ -12902,8 +13567,17 @@
       <c r="L210">
         <v>338</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M210" t="s">
+        <v>111</v>
+      </c>
+      <c r="N210" t="s">
+        <v>111</v>
+      </c>
+      <c r="O210" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>77</v>
       </c>
@@ -12941,7 +13615,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>77</v>
       </c>
@@ -12979,7 +13653,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>78</v>
       </c>
@@ -13016,8 +13690,17 @@
       <c r="L213">
         <v>101</v>
       </c>
-    </row>
-    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M213" t="s">
+        <v>110</v>
+      </c>
+      <c r="N213" t="s">
+        <v>110</v>
+      </c>
+      <c r="O213" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>78</v>
       </c>
@@ -13055,7 +13738,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>78</v>
       </c>
@@ -13093,7 +13776,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>79</v>
       </c>
@@ -13128,7 +13811,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>79</v>
       </c>
@@ -13163,7 +13846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>80</v>
       </c>
@@ -13180,7 +13863,7 @@
         <v>5.3123283666666701E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>81</v>
       </c>
@@ -13197,7 +13880,7 @@
         <v>6.3100991777777796E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>82</v>
       </c>
@@ -13214,7 +13897,7 @@
         <v>7.1304321611111096E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>83</v>
       </c>
@@ -13231,7 +13914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>84</v>
       </c>
@@ -13248,7 +13931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>85</v>
       </c>
@@ -13521,10 +14204,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L217">
-    <filterColumn colId="9">
+  <autoFilter ref="A1:O217">
+    <filterColumn colId="8">
       <filters>
         <filter val="true"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters blank="1">
+        <filter val="falso ojo"/>
+        <filter val="invalido"/>
+        <filter val="iris"/>
+        <filter val="mayor"/>
+        <filter val="parcial"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -13541,7 +14233,7 @@
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -13588,7 +14280,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -13635,7 +14327,7 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -13682,7 +14374,7 @@
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -13729,7 +14421,7 @@
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -13772,11 +14464,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
Agregados gráficos con inválidos
</commit_message>
<xml_diff>
--- a/workspace/retinoblastomaSpringApp/dataPlusPlus.xlsx
+++ b/workspace/retinoblastomaSpringApp/dataPlusPlus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="dataPlusPlus" sheetId="1" r:id="rId1"/>
@@ -14,16 +14,18 @@
     <sheet name="positivos automatico" sheetId="4" r:id="rId5"/>
     <sheet name="positivos optimos" sheetId="3" r:id="rId6"/>
     <sheet name="positivos total" sheetId="2" r:id="rId7"/>
+    <sheet name="Neg auto con inv" sheetId="9" r:id="rId8"/>
+    <sheet name="pos auto con inv" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataPlusPlus!$A$1:$O$217</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="115">
   <si>
     <t>Archivo</t>
   </si>
@@ -359,6 +361,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>promedio negativos automático con inválidos</t>
+  </si>
+  <si>
+    <t>promedio positivos automático con inválidos</t>
+  </si>
+  <si>
+    <t>Positivos automático con invalidos</t>
   </si>
 </sst>
 </file>
@@ -1272,6 +1283,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1345,6 +1357,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId2"/>
 </c:chartSpace>
 </file>
 
@@ -1828,6 +1841,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2131,6 +2145,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2259,6 +2274,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2541,6 +2557,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2614,6 +2631,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId2"/>
 </c:chartSpace>
 </file>
 
@@ -2664,6 +2682,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2946,6 +2965,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3428,6 +3448,864 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400"/>
+              <a:t>Detección automática </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400" baseline="0"/>
+              <a:t>en casos </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>negativos</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR" sz="1400" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11734711286089239"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Neg auto con inv'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>promedio negativos automático con inválidos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.516010498687664E-2"/>
+                  <c:y val="0.13608960338291043"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11369838145231841"/>
+                  <c:y val="3.9548337707786527E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Neg auto con inv'!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Blanco</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Negro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rojo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Amarillo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Neg auto con inv'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.4367707925925903E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43179902937037001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46510080177777802</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8732460925925901E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400"/>
+              <a:t>Detección automática en</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" sz="1400" baseline="0"/>
+              <a:t> casos positivos</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pos auto con inv'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Positivos automático con invalidos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.9809492563429619E-2"/>
+                  <c:y val="0.11825204141149023"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'pos auto con inv'!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Blanco</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Negro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rojo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Amarillo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pos auto con inv'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.317717316697674</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29240061974418602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35997411255813999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9907950976744199E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3465,7 +4343,158 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.29375</cdr:x>
+      <cdr:y>0.08681</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.73542</cdr:x>
+      <cdr:y>0.1875</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="1 CuadroTexto"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1343026" y="238125"/>
+          <a:ext cx="2019300" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="95000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sin detecciones</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1000" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="95000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>inválidas</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3502,7 +4531,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3539,7 +4568,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3576,7 +4605,185 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.29861</cdr:x>
+      <cdr:y>0.08449</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.74028</cdr:x>
+      <cdr:y>0.18519</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="1 CuadroTexto"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1365250" y="231775"/>
+          <a:ext cx="2019300" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="95000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sin detecciones</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1000" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="95000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>inválidas</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3613,7 +4820,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3632,6 +4839,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Gráfico 3"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3903,7 +5147,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5169,13 +6413,517 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride6.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4472C4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride7.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4472C4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O239"/>
+  <dimension ref="A1:O242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="E242" sqref="E242:H242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14201,6 +15949,40 @@
       </c>
       <c r="H239">
         <v>4.6161660454545504E-3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>112</v>
+      </c>
+      <c r="E241">
+        <v>3.4367707925925903E-2</v>
+      </c>
+      <c r="F241">
+        <v>0.43179902937037001</v>
+      </c>
+      <c r="G241">
+        <v>0.46510080177777802</v>
+      </c>
+      <c r="H241">
+        <v>6.8732460925925901E-2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>113</v>
+      </c>
+      <c r="E242">
+        <v>0.317717316697674</v>
+      </c>
+      <c r="F242">
+        <v>0.29240061974418602</v>
+      </c>
+      <c r="G242">
+        <v>0.35997411255813999</v>
+      </c>
+      <c r="H242">
+        <v>2.9907950976744199E-2</v>
       </c>
     </row>
   </sheetData>
@@ -14230,7 +16012,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14324,7 +16106,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14371,7 +16153,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14465,7 +16247,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14505,4 +16287,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2">
+        <v>3.4367707925925903E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.43179902937037001</v>
+      </c>
+      <c r="D2">
+        <v>0.46510080177777802</v>
+      </c>
+      <c r="E2">
+        <v>6.8732460925925901E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2">
+        <v>0.317717316697674</v>
+      </c>
+      <c r="C2">
+        <v>0.29240061974418602</v>
+      </c>
+      <c r="D2">
+        <v>0.35997411255813999</v>
+      </c>
+      <c r="E2">
+        <v>2.9907950976744199E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>